<commit_message>
Duong code more functions
</commit_message>
<xml_diff>
--- a/SEP_490/SaoKim_Ecommerce/SaoKim_ecommerce_BE/wwwroot/templates/receiving_template.xlsx
+++ b/SEP_490/SaoKim_Ecommerce/SaoKim_ecommerce_BE/wwwroot/templates/receiving_template.xlsx
@@ -27,9 +27,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Test receiving_template</t>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>ReceiptDate</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Uom</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
   </si>
 </sst>
 </file>
@@ -1182,17 +1200,44 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="24.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="19.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="49.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="15.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="18.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="15.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SignalR for full warehousedashboard
</commit_message>
<xml_diff>
--- a/SEP_490/SaoKim_Ecommerce/SaoKim_ecommerce_BE/wwwroot/templates/receiving_template.xlsx
+++ b/SEP_490/SaoKim_Ecommerce/SaoKim_ecommerce_BE/wwwroot/templates/receiving_template.xlsx
@@ -27,9 +27,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Test receiving_template</t>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>ReceiptDate</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Uom</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
   </si>
 </sst>
 </file>
@@ -1182,17 +1200,44 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="24.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="19.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="49.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="15.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="18.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="15.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>